<commit_message>
Adding attempt to load data from MS CSV
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="70">
   <si>
     <t>Data</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>2020-04-03</t>
+  </si>
+  <si>
+    <t>2020-04-04</t>
   </si>
   <si>
     <t>UF</t>
@@ -554,7 +557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB40"/>
+  <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4000,6 +4003,92 @@
         <v>12</v>
       </c>
     </row>
+    <row r="41" spans="1:28">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41">
+        <v>46</v>
+      </c>
+      <c r="C41">
+        <v>23</v>
+      </c>
+      <c r="D41">
+        <v>28</v>
+      </c>
+      <c r="E41">
+        <v>311</v>
+      </c>
+      <c r="F41">
+        <v>332</v>
+      </c>
+      <c r="G41">
+        <v>730</v>
+      </c>
+      <c r="H41">
+        <v>454</v>
+      </c>
+      <c r="I41">
+        <v>153</v>
+      </c>
+      <c r="J41">
+        <v>103</v>
+      </c>
+      <c r="K41">
+        <v>88</v>
+      </c>
+      <c r="L41">
+        <v>56</v>
+      </c>
+      <c r="M41">
+        <v>62</v>
+      </c>
+      <c r="N41">
+        <v>430</v>
+      </c>
+      <c r="O41">
+        <v>80</v>
+      </c>
+      <c r="P41">
+        <v>32</v>
+      </c>
+      <c r="Q41">
+        <v>395</v>
+      </c>
+      <c r="R41">
+        <v>176</v>
+      </c>
+      <c r="S41">
+        <v>22</v>
+      </c>
+      <c r="T41">
+        <v>1246</v>
+      </c>
+      <c r="U41">
+        <v>212</v>
+      </c>
+      <c r="V41">
+        <v>410</v>
+      </c>
+      <c r="W41">
+        <v>11</v>
+      </c>
+      <c r="X41">
+        <v>37</v>
+      </c>
+      <c r="Y41">
+        <v>334</v>
+      </c>
+      <c r="Z41">
+        <v>4466</v>
+      </c>
+      <c r="AA41">
+        <v>27</v>
+      </c>
+      <c r="AB41">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4007,7 +4096,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB40"/>
+  <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7450,6 +7539,92 @@
         <v>2</v>
       </c>
       <c r="AB40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>12</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+      <c r="G41">
+        <v>22</v>
+      </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>6</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>2</v>
+      </c>
+      <c r="Q41">
+        <v>6</v>
+      </c>
+      <c r="R41">
+        <v>14</v>
+      </c>
+      <c r="S41">
+        <v>4</v>
+      </c>
+      <c r="T41">
+        <v>58</v>
+      </c>
+      <c r="U41">
+        <v>5</v>
+      </c>
+      <c r="V41">
+        <v>6</v>
+      </c>
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="X41">
+        <v>1</v>
+      </c>
+      <c r="Y41">
+        <v>5</v>
+      </c>
+      <c r="Z41">
+        <v>260</v>
+      </c>
+      <c r="AA41">
+        <v>2</v>
+      </c>
+      <c r="AB41">
         <v>0</v>
       </c>
     </row>
@@ -7468,10 +7643,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Adding data summaries, styling, deal with corrupted MS data
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="71">
   <si>
     <t>Data</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>2020-04-04</t>
+  </si>
+  <si>
+    <t>2020-04-05</t>
   </si>
   <si>
     <t>UF</t>
@@ -557,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB41"/>
+  <dimension ref="A1:AB42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4089,6 +4092,92 @@
         <v>14</v>
       </c>
     </row>
+    <row r="42" spans="1:28">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>28</v>
+      </c>
+      <c r="D42">
+        <v>29</v>
+      </c>
+      <c r="E42">
+        <v>417</v>
+      </c>
+      <c r="F42">
+        <v>401</v>
+      </c>
+      <c r="G42">
+        <v>823</v>
+      </c>
+      <c r="H42">
+        <v>468</v>
+      </c>
+      <c r="I42">
+        <v>166</v>
+      </c>
+      <c r="J42">
+        <v>115</v>
+      </c>
+      <c r="K42">
+        <v>96</v>
+      </c>
+      <c r="L42">
+        <v>60</v>
+      </c>
+      <c r="M42">
+        <v>65</v>
+      </c>
+      <c r="N42">
+        <v>498</v>
+      </c>
+      <c r="O42">
+        <v>86</v>
+      </c>
+      <c r="P42">
+        <v>34</v>
+      </c>
+      <c r="Q42">
+        <v>438</v>
+      </c>
+      <c r="R42">
+        <v>201</v>
+      </c>
+      <c r="S42">
+        <v>23</v>
+      </c>
+      <c r="T42">
+        <v>1394</v>
+      </c>
+      <c r="U42">
+        <v>242</v>
+      </c>
+      <c r="V42">
+        <v>418</v>
+      </c>
+      <c r="W42">
+        <v>12</v>
+      </c>
+      <c r="X42">
+        <v>42</v>
+      </c>
+      <c r="Y42">
+        <v>357</v>
+      </c>
+      <c r="Z42">
+        <v>4620</v>
+      </c>
+      <c r="AA42">
+        <v>32</v>
+      </c>
+      <c r="AB42">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4096,7 +4185,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB41"/>
+  <dimension ref="A1:AB42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7625,6 +7714,92 @@
         <v>2</v>
       </c>
       <c r="AB41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>14</v>
+      </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>26</v>
+      </c>
+      <c r="H42">
+        <v>7</v>
+      </c>
+      <c r="I42">
+        <v>6</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+      <c r="K42">
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>6</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42">
+        <v>4</v>
+      </c>
+      <c r="Q42">
+        <v>9</v>
+      </c>
+      <c r="R42">
+        <v>21</v>
+      </c>
+      <c r="S42">
+        <v>4</v>
+      </c>
+      <c r="T42">
+        <v>64</v>
+      </c>
+      <c r="U42">
+        <v>7</v>
+      </c>
+      <c r="V42">
+        <v>7</v>
+      </c>
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42">
+        <v>1</v>
+      </c>
+      <c r="Y42">
+        <v>10</v>
+      </c>
+      <c r="Z42">
+        <v>275</v>
+      </c>
+      <c r="AA42">
+        <v>3</v>
+      </c>
+      <c r="AB42">
         <v>0</v>
       </c>
     </row>
@@ -7643,10 +7818,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Update MS data checking
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="74">
   <si>
     <t>Data</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>2020-04-07</t>
+  </si>
+  <si>
+    <t>2020-04-08</t>
   </si>
   <si>
     <t>UF</t>
@@ -566,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB44"/>
+  <dimension ref="A1:AB45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4356,6 +4359,92 @@
         <v>19</v>
       </c>
     </row>
+    <row r="45" spans="1:28">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45">
+        <v>54</v>
+      </c>
+      <c r="C45">
+        <v>37</v>
+      </c>
+      <c r="D45">
+        <v>107</v>
+      </c>
+      <c r="E45">
+        <v>804</v>
+      </c>
+      <c r="F45">
+        <v>497</v>
+      </c>
+      <c r="G45">
+        <v>1291</v>
+      </c>
+      <c r="H45">
+        <v>509</v>
+      </c>
+      <c r="I45">
+        <v>227</v>
+      </c>
+      <c r="J45">
+        <v>158</v>
+      </c>
+      <c r="K45">
+        <v>230</v>
+      </c>
+      <c r="L45">
+        <v>90</v>
+      </c>
+      <c r="M45">
+        <v>85</v>
+      </c>
+      <c r="N45">
+        <v>614</v>
+      </c>
+      <c r="O45">
+        <v>167</v>
+      </c>
+      <c r="P45">
+        <v>41</v>
+      </c>
+      <c r="Q45">
+        <v>539</v>
+      </c>
+      <c r="R45">
+        <v>401</v>
+      </c>
+      <c r="S45">
+        <v>31</v>
+      </c>
+      <c r="T45">
+        <v>1938</v>
+      </c>
+      <c r="U45">
+        <v>261</v>
+      </c>
+      <c r="V45">
+        <v>555</v>
+      </c>
+      <c r="W45">
+        <v>18</v>
+      </c>
+      <c r="X45">
+        <v>49</v>
+      </c>
+      <c r="Y45">
+        <v>457</v>
+      </c>
+      <c r="Z45">
+        <v>6708</v>
+      </c>
+      <c r="AA45">
+        <v>36</v>
+      </c>
+      <c r="AB45">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4363,7 +4452,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB44"/>
+  <dimension ref="A1:AB45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8150,6 +8239,92 @@
         <v>4</v>
       </c>
       <c r="AB44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>30</v>
+      </c>
+      <c r="F45">
+        <v>15</v>
+      </c>
+      <c r="G45">
+        <v>43</v>
+      </c>
+      <c r="H45">
+        <v>12</v>
+      </c>
+      <c r="I45">
+        <v>6</v>
+      </c>
+      <c r="J45">
+        <v>7</v>
+      </c>
+      <c r="K45">
+        <v>11</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>2</v>
+      </c>
+      <c r="N45">
+        <v>14</v>
+      </c>
+      <c r="O45">
+        <v>6</v>
+      </c>
+      <c r="P45">
+        <v>4</v>
+      </c>
+      <c r="Q45">
+        <v>17</v>
+      </c>
+      <c r="R45">
+        <v>46</v>
+      </c>
+      <c r="S45">
+        <v>5</v>
+      </c>
+      <c r="T45">
+        <v>106</v>
+      </c>
+      <c r="U45">
+        <v>11</v>
+      </c>
+      <c r="V45">
+        <v>9</v>
+      </c>
+      <c r="W45">
+        <v>1</v>
+      </c>
+      <c r="X45">
+        <v>1</v>
+      </c>
+      <c r="Y45">
+        <v>15</v>
+      </c>
+      <c r="Z45">
+        <v>428</v>
+      </c>
+      <c r="AA45">
+        <v>4</v>
+      </c>
+      <c r="AB45">
         <v>0</v>
       </c>
     </row>
@@ -8168,10 +8343,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Add dup time plot, manual update data
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
   <si>
     <t>Data</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>2020-04-09</t>
+  </si>
+  <si>
+    <t>2020-04-10</t>
   </si>
   <si>
     <t>UF</t>
@@ -572,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB46"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4534,6 +4537,92 @@
         <v>23</v>
       </c>
     </row>
+    <row r="47" spans="1:28">
+      <c r="A47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47">
+        <v>70</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="D47">
+        <v>166</v>
+      </c>
+      <c r="E47">
+        <v>981</v>
+      </c>
+      <c r="F47">
+        <v>604</v>
+      </c>
+      <c r="G47">
+        <v>1478</v>
+      </c>
+      <c r="H47">
+        <v>555</v>
+      </c>
+      <c r="I47">
+        <v>300</v>
+      </c>
+      <c r="J47">
+        <v>191</v>
+      </c>
+      <c r="K47">
+        <v>293</v>
+      </c>
+      <c r="L47">
+        <v>112</v>
+      </c>
+      <c r="M47">
+        <v>97</v>
+      </c>
+      <c r="N47">
+        <v>698</v>
+      </c>
+      <c r="O47">
+        <v>170</v>
+      </c>
+      <c r="P47">
+        <v>79</v>
+      </c>
+      <c r="Q47">
+        <v>643</v>
+      </c>
+      <c r="R47">
+        <v>684</v>
+      </c>
+      <c r="S47">
+        <v>40</v>
+      </c>
+      <c r="T47">
+        <v>2464</v>
+      </c>
+      <c r="U47">
+        <v>263</v>
+      </c>
+      <c r="V47">
+        <v>636</v>
+      </c>
+      <c r="W47">
+        <v>32</v>
+      </c>
+      <c r="X47">
+        <v>63</v>
+      </c>
+      <c r="Y47">
+        <v>693</v>
+      </c>
+      <c r="Z47">
+        <v>8216</v>
+      </c>
+      <c r="AA47">
+        <v>42</v>
+      </c>
+      <c r="AB47">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4541,7 +4630,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB46"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8500,6 +8589,92 @@
         <v>4</v>
       </c>
       <c r="AB46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
+      <c r="A47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>50</v>
+      </c>
+      <c r="F47">
+        <v>19</v>
+      </c>
+      <c r="G47">
+        <v>58</v>
+      </c>
+      <c r="H47">
+        <v>14</v>
+      </c>
+      <c r="I47">
+        <v>7</v>
+      </c>
+      <c r="J47">
+        <v>8</v>
+      </c>
+      <c r="K47">
+        <v>16</v>
+      </c>
+      <c r="L47">
+        <v>2</v>
+      </c>
+      <c r="M47">
+        <v>2</v>
+      </c>
+      <c r="N47">
+        <v>17</v>
+      </c>
+      <c r="O47">
+        <v>9</v>
+      </c>
+      <c r="P47">
+        <v>11</v>
+      </c>
+      <c r="Q47">
+        <v>25</v>
+      </c>
+      <c r="R47">
+        <v>65</v>
+      </c>
+      <c r="S47">
+        <v>7</v>
+      </c>
+      <c r="T47">
+        <v>147</v>
+      </c>
+      <c r="U47">
+        <v>11</v>
+      </c>
+      <c r="V47">
+        <v>14</v>
+      </c>
+      <c r="W47">
+        <v>2</v>
+      </c>
+      <c r="X47">
+        <v>3</v>
+      </c>
+      <c r="Y47">
+        <v>18</v>
+      </c>
+      <c r="Z47">
+        <v>540</v>
+      </c>
+      <c r="AA47">
+        <v>4</v>
+      </c>
+      <c r="AB47">
         <v>0</v>
       </c>
     </row>
@@ -8518,10 +8693,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Fixing world deaths bug; updating data
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="78">
   <si>
     <t>Data</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>2020-04-10</t>
+  </si>
+  <si>
+    <t>2020-04-11</t>
+  </si>
+  <si>
+    <t>2020-04-12</t>
   </si>
   <si>
     <t>UF</t>
@@ -575,7 +581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB47"/>
+  <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4623,6 +4629,178 @@
         <v>23</v>
       </c>
     </row>
+    <row r="48" spans="1:28">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48">
+        <v>72</v>
+      </c>
+      <c r="C48">
+        <v>48</v>
+      </c>
+      <c r="D48">
+        <v>193</v>
+      </c>
+      <c r="E48">
+        <v>1050</v>
+      </c>
+      <c r="F48">
+        <v>635</v>
+      </c>
+      <c r="G48">
+        <v>1582</v>
+      </c>
+      <c r="H48">
+        <v>579</v>
+      </c>
+      <c r="I48">
+        <v>349</v>
+      </c>
+      <c r="J48">
+        <v>209</v>
+      </c>
+      <c r="K48">
+        <v>344</v>
+      </c>
+      <c r="L48">
+        <v>121</v>
+      </c>
+      <c r="M48">
+        <v>100</v>
+      </c>
+      <c r="N48">
+        <v>750</v>
+      </c>
+      <c r="O48">
+        <v>217</v>
+      </c>
+      <c r="P48">
+        <v>85</v>
+      </c>
+      <c r="Q48">
+        <v>676</v>
+      </c>
+      <c r="R48">
+        <v>816</v>
+      </c>
+      <c r="S48">
+        <v>41</v>
+      </c>
+      <c r="T48">
+        <v>2607</v>
+      </c>
+      <c r="U48">
+        <v>289</v>
+      </c>
+      <c r="V48">
+        <v>640</v>
+      </c>
+      <c r="W48">
+        <v>33</v>
+      </c>
+      <c r="X48">
+        <v>75</v>
+      </c>
+      <c r="Y48">
+        <v>732</v>
+      </c>
+      <c r="Z48">
+        <v>8419</v>
+      </c>
+      <c r="AA48">
+        <v>42</v>
+      </c>
+      <c r="AB48">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28">
+      <c r="A49" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49">
+        <v>77</v>
+      </c>
+      <c r="C49">
+        <v>48</v>
+      </c>
+      <c r="D49">
+        <v>230</v>
+      </c>
+      <c r="E49">
+        <v>1206</v>
+      </c>
+      <c r="F49">
+        <v>673</v>
+      </c>
+      <c r="G49">
+        <v>1676</v>
+      </c>
+      <c r="H49">
+        <v>614</v>
+      </c>
+      <c r="I49">
+        <v>383</v>
+      </c>
+      <c r="J49">
+        <v>229</v>
+      </c>
+      <c r="K49">
+        <v>398</v>
+      </c>
+      <c r="L49">
+        <v>123</v>
+      </c>
+      <c r="M49">
+        <v>101</v>
+      </c>
+      <c r="N49">
+        <v>806</v>
+      </c>
+      <c r="O49">
+        <v>246</v>
+      </c>
+      <c r="P49">
+        <v>101</v>
+      </c>
+      <c r="Q49">
+        <v>738</v>
+      </c>
+      <c r="R49">
+        <v>960</v>
+      </c>
+      <c r="S49">
+        <v>44</v>
+      </c>
+      <c r="T49">
+        <v>2855</v>
+      </c>
+      <c r="U49">
+        <v>302</v>
+      </c>
+      <c r="V49">
+        <v>653</v>
+      </c>
+      <c r="W49">
+        <v>35</v>
+      </c>
+      <c r="X49">
+        <v>79</v>
+      </c>
+      <c r="Y49">
+        <v>768</v>
+      </c>
+      <c r="Z49">
+        <v>8755</v>
+      </c>
+      <c r="AA49">
+        <v>44</v>
+      </c>
+      <c r="AB49">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4630,7 +4808,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB47"/>
+  <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8675,6 +8853,178 @@
         <v>4</v>
       </c>
       <c r="AB47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>53</v>
+      </c>
+      <c r="F48">
+        <v>21</v>
+      </c>
+      <c r="G48">
+        <v>67</v>
+      </c>
+      <c r="H48">
+        <v>14</v>
+      </c>
+      <c r="I48">
+        <v>9</v>
+      </c>
+      <c r="J48">
+        <v>10</v>
+      </c>
+      <c r="K48">
+        <v>21</v>
+      </c>
+      <c r="L48">
+        <v>3</v>
+      </c>
+      <c r="M48">
+        <v>2</v>
+      </c>
+      <c r="N48">
+        <v>17</v>
+      </c>
+      <c r="O48">
+        <v>10</v>
+      </c>
+      <c r="P48">
+        <v>11</v>
+      </c>
+      <c r="Q48">
+        <v>26</v>
+      </c>
+      <c r="R48">
+        <v>72</v>
+      </c>
+      <c r="S48">
+        <v>7</v>
+      </c>
+      <c r="T48">
+        <v>155</v>
+      </c>
+      <c r="U48">
+        <v>13</v>
+      </c>
+      <c r="V48">
+        <v>15</v>
+      </c>
+      <c r="W48">
+        <v>2</v>
+      </c>
+      <c r="X48">
+        <v>3</v>
+      </c>
+      <c r="Y48">
+        <v>21</v>
+      </c>
+      <c r="Z48">
+        <v>560</v>
+      </c>
+      <c r="AA48">
+        <v>4</v>
+      </c>
+      <c r="AB48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28">
+      <c r="A49" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>62</v>
+      </c>
+      <c r="F49">
+        <v>21</v>
+      </c>
+      <c r="G49">
+        <v>74</v>
+      </c>
+      <c r="H49">
+        <v>14</v>
+      </c>
+      <c r="I49">
+        <v>9</v>
+      </c>
+      <c r="J49">
+        <v>14</v>
+      </c>
+      <c r="K49">
+        <v>24</v>
+      </c>
+      <c r="L49">
+        <v>3</v>
+      </c>
+      <c r="M49">
+        <v>2</v>
+      </c>
+      <c r="N49">
+        <v>20</v>
+      </c>
+      <c r="O49">
+        <v>13</v>
+      </c>
+      <c r="P49">
+        <v>13</v>
+      </c>
+      <c r="Q49">
+        <v>30</v>
+      </c>
+      <c r="R49">
+        <v>85</v>
+      </c>
+      <c r="S49">
+        <v>7</v>
+      </c>
+      <c r="T49">
+        <v>170</v>
+      </c>
+      <c r="U49">
+        <v>15</v>
+      </c>
+      <c r="V49">
+        <v>16</v>
+      </c>
+      <c r="W49">
+        <v>2</v>
+      </c>
+      <c r="X49">
+        <v>3</v>
+      </c>
+      <c r="Y49">
+        <v>24</v>
+      </c>
+      <c r="Z49">
+        <v>588</v>
+      </c>
+      <c r="AA49">
+        <v>4</v>
+      </c>
+      <c r="AB49">
         <v>0</v>
       </c>
     </row>
@@ -8693,10 +9043,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Removing region plots;adding DBL of states;updating data
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
   <si>
     <t>Data</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>2020-04-12</t>
+  </si>
+  <si>
+    <t>2020-04-13</t>
   </si>
   <si>
     <t>UF</t>
@@ -581,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB49"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4801,6 +4804,92 @@
         <v>25</v>
       </c>
     </row>
+    <row r="50" spans="1:28">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50">
+        <v>90</v>
+      </c>
+      <c r="C50">
+        <v>50</v>
+      </c>
+      <c r="D50">
+        <v>242</v>
+      </c>
+      <c r="E50">
+        <v>1275</v>
+      </c>
+      <c r="F50">
+        <v>723</v>
+      </c>
+      <c r="G50">
+        <v>1800</v>
+      </c>
+      <c r="H50">
+        <v>638</v>
+      </c>
+      <c r="I50">
+        <v>430</v>
+      </c>
+      <c r="J50">
+        <v>233</v>
+      </c>
+      <c r="K50">
+        <v>445</v>
+      </c>
+      <c r="L50">
+        <v>134</v>
+      </c>
+      <c r="M50">
+        <v>113</v>
+      </c>
+      <c r="N50">
+        <v>815</v>
+      </c>
+      <c r="O50">
+        <v>270</v>
+      </c>
+      <c r="P50">
+        <v>111</v>
+      </c>
+      <c r="Q50">
+        <v>756</v>
+      </c>
+      <c r="R50">
+        <v>1154</v>
+      </c>
+      <c r="S50">
+        <v>50</v>
+      </c>
+      <c r="T50">
+        <v>3231</v>
+      </c>
+      <c r="U50">
+        <v>339</v>
+      </c>
+      <c r="V50">
+        <v>664</v>
+      </c>
+      <c r="W50">
+        <v>42</v>
+      </c>
+      <c r="X50">
+        <v>83</v>
+      </c>
+      <c r="Y50">
+        <v>777</v>
+      </c>
+      <c r="Z50">
+        <v>8895</v>
+      </c>
+      <c r="AA50">
+        <v>44</v>
+      </c>
+      <c r="AB50">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4808,7 +4897,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB49"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9025,6 +9114,92 @@
         <v>4</v>
       </c>
       <c r="AB49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>71</v>
+      </c>
+      <c r="F50">
+        <v>22</v>
+      </c>
+      <c r="G50">
+        <v>91</v>
+      </c>
+      <c r="H50">
+        <v>15</v>
+      </c>
+      <c r="I50">
+        <v>14</v>
+      </c>
+      <c r="J50">
+        <v>15</v>
+      </c>
+      <c r="K50">
+        <v>27</v>
+      </c>
+      <c r="L50">
+        <v>4</v>
+      </c>
+      <c r="M50">
+        <v>4</v>
+      </c>
+      <c r="N50">
+        <v>23</v>
+      </c>
+      <c r="O50">
+        <v>15</v>
+      </c>
+      <c r="P50">
+        <v>13</v>
+      </c>
+      <c r="Q50">
+        <v>31</v>
+      </c>
+      <c r="R50">
+        <v>102</v>
+      </c>
+      <c r="S50">
+        <v>8</v>
+      </c>
+      <c r="T50">
+        <v>188</v>
+      </c>
+      <c r="U50">
+        <v>17</v>
+      </c>
+      <c r="V50">
+        <v>16</v>
+      </c>
+      <c r="W50">
+        <v>2</v>
+      </c>
+      <c r="X50">
+        <v>3</v>
+      </c>
+      <c r="Y50">
+        <v>24</v>
+      </c>
+      <c r="Z50">
+        <v>608</v>
+      </c>
+      <c r="AA50">
+        <v>4</v>
+      </c>
+      <c r="AB50">
         <v>0</v>
       </c>
     </row>
@@ -9043,10 +9218,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Update data and data checking rules
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="80">
   <si>
     <t>Data</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>2020-04-13</t>
+  </si>
+  <si>
+    <t>2020-04-14</t>
   </si>
   <si>
     <t>UF</t>
@@ -584,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB50"/>
+  <dimension ref="A1:AB51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4890,6 +4893,92 @@
         <v>26</v>
       </c>
     </row>
+    <row r="51" spans="1:28">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51">
+        <v>99</v>
+      </c>
+      <c r="C51">
+        <v>72</v>
+      </c>
+      <c r="D51">
+        <v>307</v>
+      </c>
+      <c r="E51">
+        <v>1484</v>
+      </c>
+      <c r="F51">
+        <v>759</v>
+      </c>
+      <c r="G51">
+        <v>2005</v>
+      </c>
+      <c r="H51">
+        <v>651</v>
+      </c>
+      <c r="I51">
+        <v>463</v>
+      </c>
+      <c r="J51">
+        <v>284</v>
+      </c>
+      <c r="K51">
+        <v>478</v>
+      </c>
+      <c r="L51">
+        <v>138</v>
+      </c>
+      <c r="M51">
+        <v>115</v>
+      </c>
+      <c r="N51">
+        <v>884</v>
+      </c>
+      <c r="O51">
+        <v>323</v>
+      </c>
+      <c r="P51">
+        <v>136</v>
+      </c>
+      <c r="Q51">
+        <v>791</v>
+      </c>
+      <c r="R51">
+        <v>1284</v>
+      </c>
+      <c r="S51">
+        <v>58</v>
+      </c>
+      <c r="T51">
+        <v>3410</v>
+      </c>
+      <c r="U51">
+        <v>376</v>
+      </c>
+      <c r="V51">
+        <v>700</v>
+      </c>
+      <c r="W51">
+        <v>64</v>
+      </c>
+      <c r="X51">
+        <v>113</v>
+      </c>
+      <c r="Y51">
+        <v>826</v>
+      </c>
+      <c r="Z51">
+        <v>9371</v>
+      </c>
+      <c r="AA51">
+        <v>45</v>
+      </c>
+      <c r="AB51">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4897,7 +4986,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB50"/>
+  <dimension ref="A1:AB51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9200,6 +9289,92 @@
         <v>4</v>
       </c>
       <c r="AB50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>90</v>
+      </c>
+      <c r="F51">
+        <v>22</v>
+      </c>
+      <c r="G51">
+        <v>107</v>
+      </c>
+      <c r="H51">
+        <v>17</v>
+      </c>
+      <c r="I51">
+        <v>17</v>
+      </c>
+      <c r="J51">
+        <v>15</v>
+      </c>
+      <c r="K51">
+        <v>32</v>
+      </c>
+      <c r="L51">
+        <v>4</v>
+      </c>
+      <c r="M51">
+        <v>4</v>
+      </c>
+      <c r="N51">
+        <v>27</v>
+      </c>
+      <c r="O51">
+        <v>19</v>
+      </c>
+      <c r="P51">
+        <v>16</v>
+      </c>
+      <c r="Q51">
+        <v>36</v>
+      </c>
+      <c r="R51">
+        <v>115</v>
+      </c>
+      <c r="S51">
+        <v>8</v>
+      </c>
+      <c r="T51">
+        <v>224</v>
+      </c>
+      <c r="U51">
+        <v>18</v>
+      </c>
+      <c r="V51">
+        <v>18</v>
+      </c>
+      <c r="W51">
+        <v>2</v>
+      </c>
+      <c r="X51">
+        <v>3</v>
+      </c>
+      <c r="Y51">
+        <v>26</v>
+      </c>
+      <c r="Z51">
+        <v>695</v>
+      </c>
+      <c r="AA51">
+        <v>4</v>
+      </c>
+      <c r="AB51">
         <v>0</v>
       </c>
     </row>
@@ -9218,10 +9393,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Make data summary and select sticky;updating data
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="81">
   <si>
     <t>Data</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>2020-04-14</t>
+  </si>
+  <si>
+    <t>2020-04-15</t>
   </si>
   <si>
     <t>UF</t>
@@ -587,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB51"/>
+  <dimension ref="A1:AB52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4979,6 +4982,92 @@
         <v>26</v>
       </c>
     </row>
+    <row r="52" spans="1:28">
+      <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52">
+        <v>101</v>
+      </c>
+      <c r="C52">
+        <v>82</v>
+      </c>
+      <c r="D52">
+        <v>334</v>
+      </c>
+      <c r="E52">
+        <v>1554</v>
+      </c>
+      <c r="F52">
+        <v>807</v>
+      </c>
+      <c r="G52">
+        <v>2157</v>
+      </c>
+      <c r="H52">
+        <v>682</v>
+      </c>
+      <c r="I52">
+        <v>557</v>
+      </c>
+      <c r="J52">
+        <v>304</v>
+      </c>
+      <c r="K52">
+        <v>630</v>
+      </c>
+      <c r="L52">
+        <v>151</v>
+      </c>
+      <c r="M52">
+        <v>121</v>
+      </c>
+      <c r="N52">
+        <v>903</v>
+      </c>
+      <c r="O52">
+        <v>384</v>
+      </c>
+      <c r="P52">
+        <v>136</v>
+      </c>
+      <c r="Q52">
+        <v>803</v>
+      </c>
+      <c r="R52">
+        <v>1484</v>
+      </c>
+      <c r="S52">
+        <v>75</v>
+      </c>
+      <c r="T52">
+        <v>3743</v>
+      </c>
+      <c r="U52">
+        <v>399</v>
+      </c>
+      <c r="V52">
+        <v>747</v>
+      </c>
+      <c r="W52">
+        <v>69</v>
+      </c>
+      <c r="X52">
+        <v>114</v>
+      </c>
+      <c r="Y52">
+        <v>826</v>
+      </c>
+      <c r="Z52">
+        <v>11043</v>
+      </c>
+      <c r="AA52">
+        <v>46</v>
+      </c>
+      <c r="AB52">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4986,7 +5075,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB51"/>
+  <dimension ref="A1:AB52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9375,6 +9464,92 @@
         <v>4</v>
       </c>
       <c r="AB51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28">
+      <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>7</v>
+      </c>
+      <c r="E52">
+        <v>106</v>
+      </c>
+      <c r="F52">
+        <v>27</v>
+      </c>
+      <c r="G52">
+        <v>116</v>
+      </c>
+      <c r="H52">
+        <v>17</v>
+      </c>
+      <c r="I52">
+        <v>18</v>
+      </c>
+      <c r="J52">
+        <v>15</v>
+      </c>
+      <c r="K52">
+        <v>34</v>
+      </c>
+      <c r="L52">
+        <v>4</v>
+      </c>
+      <c r="M52">
+        <v>4</v>
+      </c>
+      <c r="N52">
+        <v>30</v>
+      </c>
+      <c r="O52">
+        <v>21</v>
+      </c>
+      <c r="P52">
+        <v>16</v>
+      </c>
+      <c r="Q52">
+        <v>38</v>
+      </c>
+      <c r="R52">
+        <v>143</v>
+      </c>
+      <c r="S52">
+        <v>8</v>
+      </c>
+      <c r="T52">
+        <v>265</v>
+      </c>
+      <c r="U52">
+        <v>19</v>
+      </c>
+      <c r="V52">
+        <v>19</v>
+      </c>
+      <c r="W52">
+        <v>2</v>
+      </c>
+      <c r="X52">
+        <v>3</v>
+      </c>
+      <c r="Y52">
+        <v>26</v>
+      </c>
+      <c r="Z52">
+        <v>778</v>
+      </c>
+      <c r="AA52">
+        <v>4</v>
+      </c>
+      <c r="AB52">
         <v>0</v>
       </c>
     </row>
@@ -9393,10 +9568,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Update data;add plot CSS for @media
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="85">
   <si>
     <t>Data</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>2020-04-16</t>
+  </si>
+  <si>
+    <t>2020-04-17</t>
+  </si>
+  <si>
+    <t>2020-04-18</t>
+  </si>
+  <si>
+    <t>2020-04-19</t>
   </si>
   <si>
     <t>UF</t>
@@ -593,7 +602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB53"/>
+  <dimension ref="A1:AB56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5157,6 +5166,264 @@
         <v>29</v>
       </c>
     </row>
+    <row r="54" spans="1:28">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54">
+        <v>135</v>
+      </c>
+      <c r="C54">
+        <v>110</v>
+      </c>
+      <c r="D54">
+        <v>370</v>
+      </c>
+      <c r="E54">
+        <v>1809</v>
+      </c>
+      <c r="F54">
+        <v>1059</v>
+      </c>
+      <c r="G54">
+        <v>2684</v>
+      </c>
+      <c r="H54">
+        <v>746</v>
+      </c>
+      <c r="I54">
+        <v>856</v>
+      </c>
+      <c r="J54">
+        <v>335</v>
+      </c>
+      <c r="K54">
+        <v>797</v>
+      </c>
+      <c r="L54">
+        <v>162</v>
+      </c>
+      <c r="M54">
+        <v>143</v>
+      </c>
+      <c r="N54">
+        <v>1021</v>
+      </c>
+      <c r="O54">
+        <v>557</v>
+      </c>
+      <c r="P54">
+        <v>195</v>
+      </c>
+      <c r="Q54">
+        <v>874</v>
+      </c>
+      <c r="R54">
+        <v>2006</v>
+      </c>
+      <c r="S54">
+        <v>102</v>
+      </c>
+      <c r="T54">
+        <v>4349</v>
+      </c>
+      <c r="U54">
+        <v>463</v>
+      </c>
+      <c r="V54">
+        <v>802</v>
+      </c>
+      <c r="W54">
+        <v>92</v>
+      </c>
+      <c r="X54">
+        <v>164</v>
+      </c>
+      <c r="Y54">
+        <v>926</v>
+      </c>
+      <c r="Z54">
+        <v>12841</v>
+      </c>
+      <c r="AA54">
+        <v>53</v>
+      </c>
+      <c r="AB54">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55">
+        <v>142</v>
+      </c>
+      <c r="C55">
+        <v>132</v>
+      </c>
+      <c r="D55">
+        <v>393</v>
+      </c>
+      <c r="E55">
+        <v>1897</v>
+      </c>
+      <c r="F55">
+        <v>1193</v>
+      </c>
+      <c r="G55">
+        <v>3034</v>
+      </c>
+      <c r="H55">
+        <v>762</v>
+      </c>
+      <c r="I55">
+        <v>952</v>
+      </c>
+      <c r="J55">
+        <v>378</v>
+      </c>
+      <c r="K55">
+        <v>1040</v>
+      </c>
+      <c r="L55">
+        <v>171</v>
+      </c>
+      <c r="M55">
+        <v>161</v>
+      </c>
+      <c r="N55">
+        <v>1077</v>
+      </c>
+      <c r="O55">
+        <v>640</v>
+      </c>
+      <c r="P55">
+        <v>205</v>
+      </c>
+      <c r="Q55">
+        <v>945</v>
+      </c>
+      <c r="R55">
+        <v>2193</v>
+      </c>
+      <c r="S55">
+        <v>123</v>
+      </c>
+      <c r="T55">
+        <v>4543</v>
+      </c>
+      <c r="U55">
+        <v>516</v>
+      </c>
+      <c r="V55">
+        <v>831</v>
+      </c>
+      <c r="W55">
+        <v>110</v>
+      </c>
+      <c r="X55">
+        <v>201</v>
+      </c>
+      <c r="Y55">
+        <v>962</v>
+      </c>
+      <c r="Z55">
+        <v>13894</v>
+      </c>
+      <c r="AA55">
+        <v>71</v>
+      </c>
+      <c r="AB55">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28">
+      <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56">
+        <v>163</v>
+      </c>
+      <c r="C56">
+        <v>159</v>
+      </c>
+      <c r="D56">
+        <v>416</v>
+      </c>
+      <c r="E56">
+        <v>2044</v>
+      </c>
+      <c r="F56">
+        <v>1230</v>
+      </c>
+      <c r="G56">
+        <v>3252</v>
+      </c>
+      <c r="H56">
+        <v>827</v>
+      </c>
+      <c r="I56">
+        <v>1099</v>
+      </c>
+      <c r="J56">
+        <v>393</v>
+      </c>
+      <c r="K56">
+        <v>1205</v>
+      </c>
+      <c r="L56">
+        <v>174</v>
+      </c>
+      <c r="M56">
+        <v>168</v>
+      </c>
+      <c r="N56">
+        <v>1154</v>
+      </c>
+      <c r="O56">
+        <v>685</v>
+      </c>
+      <c r="P56">
+        <v>236</v>
+      </c>
+      <c r="Q56">
+        <v>987</v>
+      </c>
+      <c r="R56">
+        <v>2459</v>
+      </c>
+      <c r="S56">
+        <v>145</v>
+      </c>
+      <c r="T56">
+        <v>4765</v>
+      </c>
+      <c r="U56">
+        <v>531</v>
+      </c>
+      <c r="V56">
+        <v>854</v>
+      </c>
+      <c r="W56">
+        <v>128</v>
+      </c>
+      <c r="X56">
+        <v>222</v>
+      </c>
+      <c r="Y56">
+        <v>975</v>
+      </c>
+      <c r="Z56">
+        <v>14267</v>
+      </c>
+      <c r="AA56">
+        <v>83</v>
+      </c>
+      <c r="AB56">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5164,7 +5431,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB53"/>
+  <dimension ref="A1:AB56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9725,6 +9992,264 @@
         <v>4</v>
       </c>
       <c r="AB53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>10</v>
+      </c>
+      <c r="E54">
+        <v>145</v>
+      </c>
+      <c r="F54">
+        <v>36</v>
+      </c>
+      <c r="G54">
+        <v>149</v>
+      </c>
+      <c r="H54">
+        <v>20</v>
+      </c>
+      <c r="I54">
+        <v>25</v>
+      </c>
+      <c r="J54">
+        <v>16</v>
+      </c>
+      <c r="K54">
+        <v>40</v>
+      </c>
+      <c r="L54">
+        <v>5</v>
+      </c>
+      <c r="M54">
+        <v>5</v>
+      </c>
+      <c r="N54">
+        <v>35</v>
+      </c>
+      <c r="O54">
+        <v>26</v>
+      </c>
+      <c r="P54">
+        <v>26</v>
+      </c>
+      <c r="Q54">
+        <v>42</v>
+      </c>
+      <c r="R54">
+        <v>186</v>
+      </c>
+      <c r="S54">
+        <v>8</v>
+      </c>
+      <c r="T54">
+        <v>341</v>
+      </c>
+      <c r="U54">
+        <v>23</v>
+      </c>
+      <c r="V54">
+        <v>22</v>
+      </c>
+      <c r="W54">
+        <v>3</v>
+      </c>
+      <c r="X54">
+        <v>3</v>
+      </c>
+      <c r="Y54">
+        <v>30</v>
+      </c>
+      <c r="Z54">
+        <v>928</v>
+      </c>
+      <c r="AA54">
+        <v>4</v>
+      </c>
+      <c r="AB54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>10</v>
+      </c>
+      <c r="E55">
+        <v>161</v>
+      </c>
+      <c r="F55">
+        <v>37</v>
+      </c>
+      <c r="G55">
+        <v>176</v>
+      </c>
+      <c r="H55">
+        <v>24</v>
+      </c>
+      <c r="I55">
+        <v>28</v>
+      </c>
+      <c r="J55">
+        <v>18</v>
+      </c>
+      <c r="K55">
+        <v>44</v>
+      </c>
+      <c r="L55">
+        <v>5</v>
+      </c>
+      <c r="M55">
+        <v>5</v>
+      </c>
+      <c r="N55">
+        <v>39</v>
+      </c>
+      <c r="O55">
+        <v>33</v>
+      </c>
+      <c r="P55">
+        <v>26</v>
+      </c>
+      <c r="Q55">
+        <v>46</v>
+      </c>
+      <c r="R55">
+        <v>205</v>
+      </c>
+      <c r="S55">
+        <v>9</v>
+      </c>
+      <c r="T55">
+        <v>387</v>
+      </c>
+      <c r="U55">
+        <v>24</v>
+      </c>
+      <c r="V55">
+        <v>24</v>
+      </c>
+      <c r="W55">
+        <v>3</v>
+      </c>
+      <c r="X55">
+        <v>3</v>
+      </c>
+      <c r="Y55">
+        <v>31</v>
+      </c>
+      <c r="Z55">
+        <v>991</v>
+      </c>
+      <c r="AA55">
+        <v>5</v>
+      </c>
+      <c r="AB55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28">
+      <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>15</v>
+      </c>
+      <c r="D56">
+        <v>11</v>
+      </c>
+      <c r="E56">
+        <v>182</v>
+      </c>
+      <c r="F56">
+        <v>45</v>
+      </c>
+      <c r="G56">
+        <v>186</v>
+      </c>
+      <c r="H56">
+        <v>24</v>
+      </c>
+      <c r="I56">
+        <v>30</v>
+      </c>
+      <c r="J56">
+        <v>18</v>
+      </c>
+      <c r="K56">
+        <v>48</v>
+      </c>
+      <c r="L56">
+        <v>5</v>
+      </c>
+      <c r="M56">
+        <v>5</v>
+      </c>
+      <c r="N56">
+        <v>39</v>
+      </c>
+      <c r="O56">
+        <v>34</v>
+      </c>
+      <c r="P56">
+        <v>29</v>
+      </c>
+      <c r="Q56">
+        <v>48</v>
+      </c>
+      <c r="R56">
+        <v>216</v>
+      </c>
+      <c r="S56">
+        <v>10</v>
+      </c>
+      <c r="T56">
+        <v>402</v>
+      </c>
+      <c r="U56">
+        <v>25</v>
+      </c>
+      <c r="V56">
+        <v>24</v>
+      </c>
+      <c r="W56">
+        <v>4</v>
+      </c>
+      <c r="X56">
+        <v>3</v>
+      </c>
+      <c r="Y56">
+        <v>32</v>
+      </c>
+      <c r="Z56">
+        <v>1015</v>
+      </c>
+      <c r="AA56">
+        <v>5</v>
+      </c>
+      <c r="AB56">
         <v>1</v>
       </c>
     </row>
@@ -9743,10 +10268,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Update data;use acronyms on estados dbl time
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="87">
   <si>
     <t>Data</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>2020-04-20</t>
+  </si>
+  <si>
+    <t>2020-04-21</t>
   </si>
   <si>
     <t>UF</t>
@@ -605,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB57"/>
+  <dimension ref="A1:AB58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5513,6 +5516,92 @@
         <v>34</v>
       </c>
     </row>
+    <row r="58" spans="1:28">
+      <c r="A58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58">
+        <v>195</v>
+      </c>
+      <c r="C58">
+        <v>210</v>
+      </c>
+      <c r="D58">
+        <v>457</v>
+      </c>
+      <c r="E58">
+        <v>2270</v>
+      </c>
+      <c r="F58">
+        <v>1489</v>
+      </c>
+      <c r="G58">
+        <v>3716</v>
+      </c>
+      <c r="H58">
+        <v>881</v>
+      </c>
+      <c r="I58">
+        <v>1212</v>
+      </c>
+      <c r="J58">
+        <v>421</v>
+      </c>
+      <c r="K58">
+        <v>1396</v>
+      </c>
+      <c r="L58">
+        <v>181</v>
+      </c>
+      <c r="M58">
+        <v>173</v>
+      </c>
+      <c r="N58">
+        <v>1230</v>
+      </c>
+      <c r="O58">
+        <v>1026</v>
+      </c>
+      <c r="P58">
+        <v>263</v>
+      </c>
+      <c r="Q58">
+        <v>1024</v>
+      </c>
+      <c r="R58">
+        <v>2908</v>
+      </c>
+      <c r="S58">
+        <v>186</v>
+      </c>
+      <c r="T58">
+        <v>5306</v>
+      </c>
+      <c r="U58">
+        <v>608</v>
+      </c>
+      <c r="V58">
+        <v>904</v>
+      </c>
+      <c r="W58">
+        <v>199</v>
+      </c>
+      <c r="X58">
+        <v>247</v>
+      </c>
+      <c r="Y58">
+        <v>1063</v>
+      </c>
+      <c r="Z58">
+        <v>15385</v>
+      </c>
+      <c r="AA58">
+        <v>92</v>
+      </c>
+      <c r="AB58">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5520,7 +5609,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB57"/>
+  <dimension ref="A1:AB58"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10425,6 +10514,92 @@
         <v>5</v>
       </c>
       <c r="AB57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28">
+      <c r="A58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>19</v>
+      </c>
+      <c r="D58">
+        <v>13</v>
+      </c>
+      <c r="E58">
+        <v>193</v>
+      </c>
+      <c r="F58">
+        <v>47</v>
+      </c>
+      <c r="G58">
+        <v>215</v>
+      </c>
+      <c r="H58">
+        <v>24</v>
+      </c>
+      <c r="I58">
+        <v>34</v>
+      </c>
+      <c r="J58">
+        <v>19</v>
+      </c>
+      <c r="K58">
+        <v>60</v>
+      </c>
+      <c r="L58">
+        <v>6</v>
+      </c>
+      <c r="M58">
+        <v>6</v>
+      </c>
+      <c r="N58">
+        <v>44</v>
+      </c>
+      <c r="O58">
+        <v>38</v>
+      </c>
+      <c r="P58">
+        <v>33</v>
+      </c>
+      <c r="Q58">
+        <v>51</v>
+      </c>
+      <c r="R58">
+        <v>260</v>
+      </c>
+      <c r="S58">
+        <v>14</v>
+      </c>
+      <c r="T58">
+        <v>461</v>
+      </c>
+      <c r="U58">
+        <v>28</v>
+      </c>
+      <c r="V58">
+        <v>27</v>
+      </c>
+      <c r="W58">
+        <v>4</v>
+      </c>
+      <c r="X58">
+        <v>3</v>
+      </c>
+      <c r="Y58">
+        <v>35</v>
+      </c>
+      <c r="Z58">
+        <v>1093</v>
+      </c>
+      <c r="AA58">
+        <v>5</v>
+      </c>
+      <c r="AB58">
         <v>1</v>
       </c>
     </row>
@@ -10443,10 +10618,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Updating data;adding InLoco data
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="131">
   <si>
     <t>Data</t>
   </si>
@@ -402,6 +402,9 @@
     <t>2020-05-08</t>
   </si>
   <si>
+    <t>2020-05-09</t>
+  </si>
+  <si>
     <t>UF</t>
   </si>
   <si>
@@ -737,7 +740,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB101"/>
+  <dimension ref="A1:AB102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9429,6 +9432,92 @@
         <v>423</v>
       </c>
     </row>
+    <row r="102" spans="1:28">
+      <c r="A102" t="s">
+        <v>128</v>
+      </c>
+      <c r="B102">
+        <v>1335</v>
+      </c>
+      <c r="C102">
+        <v>2172</v>
+      </c>
+      <c r="D102">
+        <v>2493</v>
+      </c>
+      <c r="E102">
+        <v>11925</v>
+      </c>
+      <c r="F102">
+        <v>5174</v>
+      </c>
+      <c r="G102">
+        <v>15879</v>
+      </c>
+      <c r="H102">
+        <v>2576</v>
+      </c>
+      <c r="I102">
+        <v>4412</v>
+      </c>
+      <c r="J102">
+        <v>1069</v>
+      </c>
+      <c r="K102">
+        <v>6765</v>
+      </c>
+      <c r="L102">
+        <v>502</v>
+      </c>
+      <c r="M102">
+        <v>346</v>
+      </c>
+      <c r="N102">
+        <v>3123</v>
+      </c>
+      <c r="O102">
+        <v>6775</v>
+      </c>
+      <c r="P102">
+        <v>2156</v>
+      </c>
+      <c r="Q102">
+        <v>1785</v>
+      </c>
+      <c r="R102">
+        <v>12470</v>
+      </c>
+      <c r="S102">
+        <v>1233</v>
+      </c>
+      <c r="T102">
+        <v>16929</v>
+      </c>
+      <c r="U102">
+        <v>1919</v>
+      </c>
+      <c r="V102">
+        <v>2493</v>
+      </c>
+      <c r="W102">
+        <v>1263</v>
+      </c>
+      <c r="X102">
+        <v>1202</v>
+      </c>
+      <c r="Y102">
+        <v>3372</v>
+      </c>
+      <c r="Z102">
+        <v>44411</v>
+      </c>
+      <c r="AA102">
+        <v>1588</v>
+      </c>
+      <c r="AB102">
+        <v>572</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9436,7 +9525,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB101"/>
+  <dimension ref="A1:AB102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -18125,6 +18214,92 @@
         <v>28</v>
       </c>
       <c r="AB101">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28">
+      <c r="A102" t="s">
+        <v>128</v>
+      </c>
+      <c r="B102">
+        <v>39</v>
+      </c>
+      <c r="C102">
+        <v>114</v>
+      </c>
+      <c r="D102">
+        <v>69</v>
+      </c>
+      <c r="E102">
+        <v>962</v>
+      </c>
+      <c r="F102">
+        <v>196</v>
+      </c>
+      <c r="G102">
+        <v>1062</v>
+      </c>
+      <c r="H102">
+        <v>39</v>
+      </c>
+      <c r="I102">
+        <v>172</v>
+      </c>
+      <c r="J102">
+        <v>47</v>
+      </c>
+      <c r="K102">
+        <v>355</v>
+      </c>
+      <c r="L102">
+        <v>16</v>
+      </c>
+      <c r="M102">
+        <v>11</v>
+      </c>
+      <c r="N102">
+        <v>118</v>
+      </c>
+      <c r="O102">
+        <v>578</v>
+      </c>
+      <c r="P102">
+        <v>124</v>
+      </c>
+      <c r="Q102">
+        <v>107</v>
+      </c>
+      <c r="R102">
+        <v>972</v>
+      </c>
+      <c r="S102">
+        <v>38</v>
+      </c>
+      <c r="T102">
+        <v>1653</v>
+      </c>
+      <c r="U102">
+        <v>87</v>
+      </c>
+      <c r="V102">
+        <v>95</v>
+      </c>
+      <c r="W102">
+        <v>41</v>
+      </c>
+      <c r="X102">
+        <v>18</v>
+      </c>
+      <c r="Y102">
+        <v>64</v>
+      </c>
+      <c r="Z102">
+        <v>3608</v>
+      </c>
+      <c r="AA102">
+        <v>33</v>
+      </c>
+      <c r="AB102">
         <v>9</v>
       </c>
     </row>
@@ -18143,10 +18318,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Update R for new MS platform data format
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="133">
   <si>
     <t>Data</t>
   </si>
@@ -408,6 +408,9 @@
     <t>2020-05-10</t>
   </si>
   <si>
+    <t>2020-05-11</t>
+  </si>
+  <si>
     <t>UF</t>
   </si>
   <si>
@@ -743,7 +746,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB103"/>
+  <dimension ref="A1:AB104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9607,6 +9610,92 @@
         <v>688</v>
       </c>
     </row>
+    <row r="104" spans="1:28">
+      <c r="A104" t="s">
+        <v>130</v>
+      </c>
+      <c r="B104">
+        <v>1460</v>
+      </c>
+      <c r="C104">
+        <v>2343</v>
+      </c>
+      <c r="D104">
+        <v>2671</v>
+      </c>
+      <c r="E104">
+        <v>12919</v>
+      </c>
+      <c r="F104">
+        <v>5808</v>
+      </c>
+      <c r="G104">
+        <v>17599</v>
+      </c>
+      <c r="H104">
+        <v>2783</v>
+      </c>
+      <c r="I104">
+        <v>4819</v>
+      </c>
+      <c r="J104">
+        <v>1100</v>
+      </c>
+      <c r="K104">
+        <v>8144</v>
+      </c>
+      <c r="L104">
+        <v>541</v>
+      </c>
+      <c r="M104">
+        <v>385</v>
+      </c>
+      <c r="N104">
+        <v>3320</v>
+      </c>
+      <c r="O104">
+        <v>7563</v>
+      </c>
+      <c r="P104">
+        <v>2525</v>
+      </c>
+      <c r="Q104">
+        <v>1849</v>
+      </c>
+      <c r="R104">
+        <v>13768</v>
+      </c>
+      <c r="S104">
+        <v>1332</v>
+      </c>
+      <c r="T104">
+        <v>17939</v>
+      </c>
+      <c r="U104">
+        <v>1989</v>
+      </c>
+      <c r="V104">
+        <v>2576</v>
+      </c>
+      <c r="W104">
+        <v>1989</v>
+      </c>
+      <c r="X104">
+        <v>1295</v>
+      </c>
+      <c r="Y104">
+        <v>3529</v>
+      </c>
+      <c r="Z104">
+        <v>46131</v>
+      </c>
+      <c r="AA104">
+        <v>1800</v>
+      </c>
+      <c r="AB104">
+        <v>747</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9614,7 +9703,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB103"/>
+  <dimension ref="A1:AB104"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -18476,6 +18565,92 @@
       </c>
       <c r="AB103">
         <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28">
+      <c r="A104" t="s">
+        <v>130</v>
+      </c>
+      <c r="B104">
+        <v>45</v>
+      </c>
+      <c r="C104">
+        <v>138</v>
+      </c>
+      <c r="D104">
+        <v>73</v>
+      </c>
+      <c r="E104">
+        <v>1035</v>
+      </c>
+      <c r="F104">
+        <v>211</v>
+      </c>
+      <c r="G104">
+        <v>1189</v>
+      </c>
+      <c r="H104">
+        <v>44</v>
+      </c>
+      <c r="I104">
+        <v>196</v>
+      </c>
+      <c r="J104">
+        <v>49</v>
+      </c>
+      <c r="K104">
+        <v>399</v>
+      </c>
+      <c r="L104">
+        <v>19</v>
+      </c>
+      <c r="M104">
+        <v>11</v>
+      </c>
+      <c r="N104">
+        <v>121</v>
+      </c>
+      <c r="O104">
+        <v>708</v>
+      </c>
+      <c r="P104">
+        <v>139</v>
+      </c>
+      <c r="Q104">
+        <v>111</v>
+      </c>
+      <c r="R104">
+        <v>1087</v>
+      </c>
+      <c r="S104">
+        <v>45</v>
+      </c>
+      <c r="T104">
+        <v>1770</v>
+      </c>
+      <c r="U104">
+        <v>92</v>
+      </c>
+      <c r="V104">
+        <v>105</v>
+      </c>
+      <c r="W104">
+        <v>92</v>
+      </c>
+      <c r="X104">
+        <v>24</v>
+      </c>
+      <c r="Y104">
+        <v>69</v>
+      </c>
+      <c r="Z104">
+        <v>3743</v>
+      </c>
+      <c r="AA104">
+        <v>37</v>
+      </c>
+      <c r="AB104">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -18493,10 +18668,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Adding FT plot test
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="152">
   <si>
     <t>Data</t>
   </si>
@@ -465,6 +465,9 @@
     <t>2020-05-29</t>
   </si>
   <si>
+    <t>2020-05-30</t>
+  </si>
+  <si>
     <t>UF</t>
   </si>
   <si>
@@ -800,7 +803,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB122"/>
+  <dimension ref="A1:AB123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -11298,6 +11301,92 @@
         <v>3611</v>
       </c>
     </row>
+    <row r="123" spans="1:28">
+      <c r="A123" t="s">
+        <v>149</v>
+      </c>
+      <c r="B123">
+        <v>6072</v>
+      </c>
+      <c r="C123">
+        <v>9223</v>
+      </c>
+      <c r="D123">
+        <v>9313</v>
+      </c>
+      <c r="E123">
+        <v>40560</v>
+      </c>
+      <c r="F123">
+        <v>17626</v>
+      </c>
+      <c r="G123">
+        <v>46506</v>
+      </c>
+      <c r="H123">
+        <v>9474</v>
+      </c>
+      <c r="I123">
+        <v>13437</v>
+      </c>
+      <c r="J123">
+        <v>3585</v>
+      </c>
+      <c r="K123">
+        <v>32620</v>
+      </c>
+      <c r="L123">
+        <v>2361</v>
+      </c>
+      <c r="M123">
+        <v>1418</v>
+      </c>
+      <c r="N123">
+        <v>9630</v>
+      </c>
+      <c r="O123">
+        <v>37296</v>
+      </c>
+      <c r="P123">
+        <v>12862</v>
+      </c>
+      <c r="Q123">
+        <v>4473</v>
+      </c>
+      <c r="R123">
+        <v>33427</v>
+      </c>
+      <c r="S123">
+        <v>4745</v>
+      </c>
+      <c r="T123">
+        <v>52420</v>
+      </c>
+      <c r="U123">
+        <v>7402</v>
+      </c>
+      <c r="V123">
+        <v>9242</v>
+      </c>
+      <c r="W123">
+        <v>7402</v>
+      </c>
+      <c r="X123">
+        <v>3299</v>
+      </c>
+      <c r="Y123">
+        <v>8778</v>
+      </c>
+      <c r="Z123">
+        <v>107142</v>
+      </c>
+      <c r="AA123">
+        <v>6805</v>
+      </c>
+      <c r="AB123">
+        <v>3981</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11305,7 +11394,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB122"/>
+  <dimension ref="A1:AB123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -21801,6 +21890,92 @@
       </c>
       <c r="AB122">
         <v>70</v>
+      </c>
+    </row>
+    <row r="123" spans="1:28">
+      <c r="A123" t="s">
+        <v>149</v>
+      </c>
+      <c r="B123">
+        <v>142</v>
+      </c>
+      <c r="C123">
+        <v>424</v>
+      </c>
+      <c r="D123">
+        <v>215</v>
+      </c>
+      <c r="E123">
+        <v>2047</v>
+      </c>
+      <c r="F123">
+        <v>638</v>
+      </c>
+      <c r="G123">
+        <v>2956</v>
+      </c>
+      <c r="H123">
+        <v>162</v>
+      </c>
+      <c r="I123">
+        <v>583</v>
+      </c>
+      <c r="J123">
+        <v>122</v>
+      </c>
+      <c r="K123">
+        <v>932</v>
+      </c>
+      <c r="L123">
+        <v>57</v>
+      </c>
+      <c r="M123">
+        <v>19</v>
+      </c>
+      <c r="N123">
+        <v>263</v>
+      </c>
+      <c r="O123">
+        <v>2900</v>
+      </c>
+      <c r="P123">
+        <v>347</v>
+      </c>
+      <c r="Q123">
+        <v>181</v>
+      </c>
+      <c r="R123">
+        <v>2740</v>
+      </c>
+      <c r="S123">
+        <v>157</v>
+      </c>
+      <c r="T123">
+        <v>5277</v>
+      </c>
+      <c r="U123">
+        <v>305</v>
+      </c>
+      <c r="V123">
+        <v>218</v>
+      </c>
+      <c r="W123">
+        <v>305</v>
+      </c>
+      <c r="X123">
+        <v>110</v>
+      </c>
+      <c r="Y123">
+        <v>136</v>
+      </c>
+      <c r="Z123">
+        <v>7532</v>
+      </c>
+      <c r="AA123">
+        <v>149</v>
+      </c>
+      <c r="AB123">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -21818,10 +21993,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Adding more countries to compare, translating, updating data
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="146">
   <si>
     <t>2020-02-25</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>2020-06-19</t>
+  </si>
+  <si>
+    <t>2020-06-20</t>
   </si>
   <si>
     <t>UF</t>
@@ -782,7 +785,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB116"/>
+  <dimension ref="A1:AB117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9345,7 +9348,7 @@
         <v>14540</v>
       </c>
       <c r="K116">
-        <v>35093</v>
+        <v>31760</v>
       </c>
       <c r="L116">
         <v>49720</v>
@@ -9354,7 +9357,7 @@
         <v>12932</v>
       </c>
       <c r="N116">
-        <v>16039</v>
+        <v>19206</v>
       </c>
       <c r="O116">
         <v>16332</v>
@@ -9363,7 +9366,7 @@
         <v>61683</v>
       </c>
       <c r="Q116">
-        <v>4666</v>
+        <v>4990</v>
       </c>
       <c r="R116">
         <v>17808</v>
@@ -9378,7 +9381,7 @@
         <v>82881</v>
       </c>
       <c r="V116">
-        <v>7956</v>
+        <v>8203</v>
       </c>
       <c r="W116">
         <v>13813</v>
@@ -9390,13 +9393,99 @@
         <v>68500</v>
       </c>
       <c r="Z116">
-        <v>8353</v>
+        <v>8725</v>
       </c>
       <c r="AA116">
         <v>14353</v>
       </c>
       <c r="AB116">
-        <v>7650</v>
+        <v>8037</v>
+      </c>
+    </row>
+    <row r="117" spans="1:28">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>215793</v>
+      </c>
+      <c r="C117">
+        <v>34238</v>
+      </c>
+      <c r="D117">
+        <v>95537</v>
+      </c>
+      <c r="E117">
+        <v>45304</v>
+      </c>
+      <c r="F117">
+        <v>32235</v>
+      </c>
+      <c r="G117">
+        <v>27698</v>
+      </c>
+      <c r="H117">
+        <v>27305</v>
+      </c>
+      <c r="I117">
+        <v>19138</v>
+      </c>
+      <c r="J117">
+        <v>15418</v>
+      </c>
+      <c r="K117">
+        <v>36521</v>
+      </c>
+      <c r="L117">
+        <v>51118</v>
+      </c>
+      <c r="M117">
+        <v>13821</v>
+      </c>
+      <c r="N117">
+        <v>19206</v>
+      </c>
+      <c r="O117">
+        <v>17108</v>
+      </c>
+      <c r="P117">
+        <v>62902</v>
+      </c>
+      <c r="Q117">
+        <v>4990</v>
+      </c>
+      <c r="R117">
+        <v>18449</v>
+      </c>
+      <c r="S117">
+        <v>92397</v>
+      </c>
+      <c r="T117">
+        <v>11263</v>
+      </c>
+      <c r="U117">
+        <v>84654</v>
+      </c>
+      <c r="V117">
+        <v>8203</v>
+      </c>
+      <c r="W117">
+        <v>14264</v>
+      </c>
+      <c r="X117">
+        <v>21574</v>
+      </c>
+      <c r="Y117">
+        <v>69673</v>
+      </c>
+      <c r="Z117">
+        <v>9262</v>
+      </c>
+      <c r="AA117">
+        <v>14952</v>
+      </c>
+      <c r="AB117">
+        <v>8037</v>
       </c>
     </row>
   </sheetData>
@@ -9406,7 +9495,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB116"/>
+  <dimension ref="A1:AB117"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17848,7 +17937,7 @@
         <v>361</v>
       </c>
       <c r="AB114">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" spans="1:28">
@@ -17954,7 +18043,7 @@
         <v>1305</v>
       </c>
       <c r="F116">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G116">
         <v>848</v>
@@ -17969,7 +18058,7 @@
         <v>289</v>
       </c>
       <c r="K116">
-        <v>724</v>
+        <v>709</v>
       </c>
       <c r="L116">
         <v>4102</v>
@@ -17978,7 +18067,7 @@
         <v>428</v>
       </c>
       <c r="N116">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="O116">
         <v>234</v>
@@ -17987,7 +18076,7 @@
         <v>2624</v>
       </c>
       <c r="Q116">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R116">
         <v>426</v>
@@ -18002,7 +18091,7 @@
         <v>4519</v>
       </c>
       <c r="V116">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="W116">
         <v>459</v>
@@ -18014,13 +18103,99 @@
         <v>1645</v>
       </c>
       <c r="Z116">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="AA116">
         <v>391</v>
       </c>
       <c r="AB116">
-        <v>239</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="117" spans="1:28">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>12494</v>
+      </c>
+      <c r="C117">
+        <v>1297</v>
+      </c>
+      <c r="D117">
+        <v>8824</v>
+      </c>
+      <c r="E117">
+        <v>1350</v>
+      </c>
+      <c r="F117">
+        <v>405</v>
+      </c>
+      <c r="G117">
+        <v>866</v>
+      </c>
+      <c r="H117">
+        <v>636</v>
+      </c>
+      <c r="I117">
+        <v>430</v>
+      </c>
+      <c r="J117">
+        <v>295</v>
+      </c>
+      <c r="K117">
+        <v>743</v>
+      </c>
+      <c r="L117">
+        <v>4148</v>
+      </c>
+      <c r="M117">
+        <v>437</v>
+      </c>
+      <c r="N117">
+        <v>697</v>
+      </c>
+      <c r="O117">
+        <v>237</v>
+      </c>
+      <c r="P117">
+        <v>2650</v>
+      </c>
+      <c r="Q117">
+        <v>43</v>
+      </c>
+      <c r="R117">
+        <v>448</v>
+      </c>
+      <c r="S117">
+        <v>5520</v>
+      </c>
+      <c r="T117">
+        <v>297</v>
+      </c>
+      <c r="U117">
+        <v>4583</v>
+      </c>
+      <c r="V117">
+        <v>167</v>
+      </c>
+      <c r="W117">
+        <v>485</v>
+      </c>
+      <c r="X117">
+        <v>353</v>
+      </c>
+      <c r="Y117">
+        <v>1684</v>
+      </c>
+      <c r="Z117">
+        <v>341</v>
+      </c>
+      <c r="AA117">
+        <v>409</v>
+      </c>
+      <c r="AB117">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -18038,15 +18213,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2">
         <v>1777225</v>
@@ -18054,7 +18229,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>881935</v>
@@ -18062,7 +18237,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B4">
         <v>4144597</v>
@@ -18070,7 +18245,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>605761</v>
@@ -18078,7 +18253,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B6">
         <v>8602865</v>
@@ -18086,7 +18261,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B7">
         <v>845731</v>
@@ -18094,7 +18269,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8">
         <v>1572866</v>
@@ -18102,7 +18277,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B9">
         <v>7075181</v>
@@ -18110,7 +18285,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B10">
         <v>3273227</v>
@@ -18118,7 +18293,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B11">
         <v>9132078</v>
@@ -18126,7 +18301,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B12">
         <v>3506853</v>
@@ -18134,7 +18309,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B13">
         <v>4018127</v>
@@ -18142,7 +18317,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B14">
         <v>9557071</v>
@@ -18150,7 +18325,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B15">
         <v>3337357</v>
@@ -18158,7 +18333,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B16">
         <v>2298696</v>
@@ -18166,7 +18341,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B17">
         <v>14873064</v>
@@ -18174,7 +18349,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B18">
         <v>21168791</v>
@@ -18182,7 +18357,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B19">
         <v>4018650</v>
@@ -18190,7 +18365,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B20">
         <v>17264943</v>
@@ -18198,7 +18373,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B21">
         <v>45919049</v>
@@ -18206,7 +18381,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B22">
         <v>11433957</v>
@@ -18214,7 +18389,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B23">
         <v>7164788</v>
@@ -18222,7 +18397,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B24">
         <v>11377239</v>
@@ -18230,7 +18405,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B25">
         <v>2778986</v>
@@ -18238,7 +18413,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B26">
         <v>3484466</v>
@@ -18246,7 +18421,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B27">
         <v>7018354</v>
@@ -18254,7 +18429,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B28">
         <v>3015268</v>

</xml_diff>

<commit_message>
Fixing FT plot and adding in-plot labels; updating data
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="161">
   <si>
     <t>2020-02-25</t>
   </si>
@@ -400,6 +400,18 @@
   </si>
   <si>
     <t>2020-07-01</t>
+  </si>
+  <si>
+    <t>2020-07-02</t>
+  </si>
+  <si>
+    <t>2020-07-03</t>
+  </si>
+  <si>
+    <t>2020-07-04</t>
+  </si>
+  <si>
+    <t>2020-07-05</t>
   </si>
   <si>
     <t>UF</t>
@@ -818,7 +830,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB128"/>
+  <dimension ref="A1:AB132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10164,7 +10176,7 @@
         <v>20742</v>
       </c>
       <c r="N125">
-        <v>28970</v>
+        <v>29784</v>
       </c>
       <c r="O125">
         <v>24364</v>
@@ -10336,7 +10348,7 @@
         <v>22877</v>
       </c>
       <c r="N127">
-        <v>31899</v>
+        <v>31964</v>
       </c>
       <c r="O127">
         <v>26354</v>
@@ -10410,7 +10422,7 @@
         <v>28171</v>
       </c>
       <c r="J128">
-        <v>26169</v>
+        <v>26145</v>
       </c>
       <c r="K128">
         <v>48175</v>
@@ -10422,7 +10434,7 @@
         <v>24225</v>
       </c>
       <c r="N128">
-        <v>31899</v>
+        <v>32962</v>
       </c>
       <c r="O128">
         <v>27279</v>
@@ -10431,10 +10443,10 @@
         <v>72284</v>
       </c>
       <c r="Q128">
-        <v>8676</v>
+        <v>9062</v>
       </c>
       <c r="R128">
-        <v>25915</v>
+        <v>26612</v>
       </c>
       <c r="S128">
         <v>114038</v>
@@ -10446,7 +10458,7 @@
         <v>108067</v>
       </c>
       <c r="V128">
-        <v>11222</v>
+        <v>11454</v>
       </c>
       <c r="W128">
         <v>23307</v>
@@ -10458,13 +10470,357 @@
         <v>83256</v>
       </c>
       <c r="Z128">
-        <v>16621</v>
+        <v>17401</v>
       </c>
       <c r="AA128">
-        <v>21462</v>
+        <v>21523</v>
       </c>
       <c r="AB128">
-        <v>15153</v>
+        <v>17583</v>
+      </c>
+    </row>
+    <row r="129" spans="1:28">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>302179</v>
+      </c>
+      <c r="C129">
+        <v>50242</v>
+      </c>
+      <c r="D129">
+        <v>116823</v>
+      </c>
+      <c r="E129">
+        <v>79349</v>
+      </c>
+      <c r="F129">
+        <v>52281</v>
+      </c>
+      <c r="G129">
+        <v>37328</v>
+      </c>
+      <c r="H129">
+        <v>50707</v>
+      </c>
+      <c r="I129">
+        <v>29195</v>
+      </c>
+      <c r="J129">
+        <v>26318</v>
+      </c>
+      <c r="K129">
+        <v>49536</v>
+      </c>
+      <c r="L129">
+        <v>61119</v>
+      </c>
+      <c r="M129">
+        <v>26304</v>
+      </c>
+      <c r="N129">
+        <v>33487</v>
+      </c>
+      <c r="O129">
+        <v>28575</v>
+      </c>
+      <c r="P129">
+        <v>73530</v>
+      </c>
+      <c r="Q129">
+        <v>9388</v>
+      </c>
+      <c r="R129">
+        <v>26612</v>
+      </c>
+      <c r="S129">
+        <v>116519</v>
+      </c>
+      <c r="T129">
+        <v>14048</v>
+      </c>
+      <c r="U129">
+        <v>110411</v>
+      </c>
+      <c r="V129">
+        <v>11736</v>
+      </c>
+      <c r="W129">
+        <v>24376</v>
+      </c>
+      <c r="X129">
+        <v>29153</v>
+      </c>
+      <c r="Y129">
+        <v>86025</v>
+      </c>
+      <c r="Z129">
+        <v>18356</v>
+      </c>
+      <c r="AA129">
+        <v>21970</v>
+      </c>
+      <c r="AB129">
+        <v>18323</v>
+      </c>
+    </row>
+    <row r="130" spans="1:28">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>310517</v>
+      </c>
+      <c r="C130">
+        <v>51689</v>
+      </c>
+      <c r="D130">
+        <v>118956</v>
+      </c>
+      <c r="E130">
+        <v>82314</v>
+      </c>
+      <c r="F130">
+        <v>53996</v>
+      </c>
+      <c r="G130">
+        <v>38404</v>
+      </c>
+      <c r="H130">
+        <v>53351</v>
+      </c>
+      <c r="I130">
+        <v>30371</v>
+      </c>
+      <c r="J130">
+        <v>27502</v>
+      </c>
+      <c r="K130">
+        <v>50765</v>
+      </c>
+      <c r="L130">
+        <v>62362</v>
+      </c>
+      <c r="M130">
+        <v>28166</v>
+      </c>
+      <c r="N130">
+        <v>33910</v>
+      </c>
+      <c r="O130">
+        <v>30261</v>
+      </c>
+      <c r="P130">
+        <v>74537</v>
+      </c>
+      <c r="Q130">
+        <v>9910</v>
+      </c>
+      <c r="R130">
+        <v>28186</v>
+      </c>
+      <c r="S130">
+        <v>118311</v>
+      </c>
+      <c r="T130">
+        <v>14112</v>
+      </c>
+      <c r="U130">
+        <v>112531</v>
+      </c>
+      <c r="V130">
+        <v>12282</v>
+      </c>
+      <c r="W130">
+        <v>25561</v>
+      </c>
+      <c r="X130">
+        <v>29574</v>
+      </c>
+      <c r="Y130">
+        <v>88214</v>
+      </c>
+      <c r="Z130">
+        <v>19540</v>
+      </c>
+      <c r="AA130">
+        <v>22241</v>
+      </c>
+      <c r="AB130">
+        <v>18769</v>
+      </c>
+    </row>
+    <row r="131" spans="1:28">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>312530</v>
+      </c>
+      <c r="C131">
+        <v>52824</v>
+      </c>
+      <c r="D131">
+        <v>120428</v>
+      </c>
+      <c r="E131">
+        <v>85485</v>
+      </c>
+      <c r="F131">
+        <v>55760</v>
+      </c>
+      <c r="G131">
+        <v>39255</v>
+      </c>
+      <c r="H131">
+        <v>55958</v>
+      </c>
+      <c r="I131">
+        <v>31619</v>
+      </c>
+      <c r="J131">
+        <v>28526</v>
+      </c>
+      <c r="K131">
+        <v>52306</v>
+      </c>
+      <c r="L131">
+        <v>63457</v>
+      </c>
+      <c r="M131">
+        <v>30570</v>
+      </c>
+      <c r="N131">
+        <v>34645</v>
+      </c>
+      <c r="O131">
+        <v>31931</v>
+      </c>
+      <c r="P131">
+        <v>75945</v>
+      </c>
+      <c r="Q131">
+        <v>10089</v>
+      </c>
+      <c r="R131">
+        <v>29761</v>
+      </c>
+      <c r="S131">
+        <v>121464</v>
+      </c>
+      <c r="T131">
+        <v>14487</v>
+      </c>
+      <c r="U131">
+        <v>113811</v>
+      </c>
+      <c r="V131">
+        <v>12475</v>
+      </c>
+      <c r="W131">
+        <v>26079</v>
+      </c>
+      <c r="X131">
+        <v>29809</v>
+      </c>
+      <c r="Y131">
+        <v>89057</v>
+      </c>
+      <c r="Z131">
+        <v>20333</v>
+      </c>
+      <c r="AA131">
+        <v>22957</v>
+      </c>
+      <c r="AB131">
+        <v>18922</v>
+      </c>
+    </row>
+    <row r="132" spans="1:28">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>320179</v>
+      </c>
+      <c r="C132">
+        <v>53393</v>
+      </c>
+      <c r="D132">
+        <v>121292</v>
+      </c>
+      <c r="E132">
+        <v>87048</v>
+      </c>
+      <c r="F132">
+        <v>57854</v>
+      </c>
+      <c r="G132">
+        <v>39935</v>
+      </c>
+      <c r="H132">
+        <v>58283</v>
+      </c>
+      <c r="I132">
+        <v>31955</v>
+      </c>
+      <c r="J132">
+        <v>28526</v>
+      </c>
+      <c r="K132">
+        <v>52728</v>
+      </c>
+      <c r="L132">
+        <v>65129</v>
+      </c>
+      <c r="M132">
+        <v>31459</v>
+      </c>
+      <c r="N132">
+        <v>34645</v>
+      </c>
+      <c r="O132">
+        <v>32969</v>
+      </c>
+      <c r="P132">
+        <v>76014</v>
+      </c>
+      <c r="Q132">
+        <v>10089</v>
+      </c>
+      <c r="R132">
+        <v>30217</v>
+      </c>
+      <c r="S132">
+        <v>121986</v>
+      </c>
+      <c r="T132">
+        <v>14622</v>
+      </c>
+      <c r="U132">
+        <v>114535</v>
+      </c>
+      <c r="V132">
+        <v>12475</v>
+      </c>
+      <c r="W132">
+        <v>26511</v>
+      </c>
+      <c r="X132">
+        <v>29883</v>
+      </c>
+      <c r="Y132">
+        <v>89714</v>
+      </c>
+      <c r="Z132">
+        <v>21081</v>
+      </c>
+      <c r="AA132">
+        <v>23479</v>
+      </c>
+      <c r="AB132">
+        <v>18922</v>
       </c>
     </row>
   </sheetData>
@@ -10474,7 +10830,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB128"/>
+  <dimension ref="A1:AB132"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -19820,7 +20176,7 @@
         <v>599</v>
       </c>
       <c r="N125">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c r="O125">
         <v>312</v>
@@ -19992,7 +20348,7 @@
         <v>649</v>
       </c>
       <c r="N127">
-        <v>1067</v>
+        <v>1072</v>
       </c>
       <c r="O127">
         <v>341</v>
@@ -20078,7 +20434,7 @@
         <v>663</v>
       </c>
       <c r="N128">
-        <v>1067</v>
+        <v>1108</v>
       </c>
       <c r="O128">
         <v>347</v>
@@ -20087,10 +20443,10 @@
         <v>2843</v>
       </c>
       <c r="Q128">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R128">
-        <v>702</v>
+        <v>725</v>
       </c>
       <c r="S128">
         <v>6203</v>
@@ -20102,7 +20458,7 @@
         <v>5004</v>
       </c>
       <c r="V128">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="W128">
         <v>697</v>
@@ -20114,13 +20470,357 @@
         <v>2081</v>
       </c>
       <c r="Z128">
-        <v>634</v>
+        <v>665</v>
       </c>
       <c r="AA128">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="AB128">
-        <v>314</v>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="129" spans="1:28">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>15351</v>
+      </c>
+      <c r="C129">
+        <v>1727</v>
+      </c>
+      <c r="D129">
+        <v>10332</v>
+      </c>
+      <c r="E129">
+        <v>1947</v>
+      </c>
+      <c r="F129">
+        <v>631</v>
+      </c>
+      <c r="G129">
+        <v>1091</v>
+      </c>
+      <c r="H129">
+        <v>1059</v>
+      </c>
+      <c r="I129">
+        <v>663</v>
+      </c>
+      <c r="J129">
+        <v>572</v>
+      </c>
+      <c r="K129">
+        <v>1044</v>
+      </c>
+      <c r="L129">
+        <v>4968</v>
+      </c>
+      <c r="M129">
+        <v>706</v>
+      </c>
+      <c r="N129">
+        <v>1177</v>
+      </c>
+      <c r="O129">
+        <v>362</v>
+      </c>
+      <c r="P129">
+        <v>2862</v>
+      </c>
+      <c r="Q129">
+        <v>107</v>
+      </c>
+      <c r="R129">
+        <v>725</v>
+      </c>
+      <c r="S129">
+        <v>6307</v>
+      </c>
+      <c r="T129">
+        <v>378</v>
+      </c>
+      <c r="U129">
+        <v>5050</v>
+      </c>
+      <c r="V129">
+        <v>211</v>
+      </c>
+      <c r="W129">
+        <v>726</v>
+      </c>
+      <c r="X129">
+        <v>427</v>
+      </c>
+      <c r="Y129">
+        <v>2119</v>
+      </c>
+      <c r="Z129">
+        <v>706</v>
+      </c>
+      <c r="AA129">
+        <v>530</v>
+      </c>
+      <c r="AB129">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="130" spans="1:28">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>15694</v>
+      </c>
+      <c r="C130">
+        <v>1758</v>
+      </c>
+      <c r="D130">
+        <v>10500</v>
+      </c>
+      <c r="E130">
+        <v>2001</v>
+      </c>
+      <c r="F130">
+        <v>643</v>
+      </c>
+      <c r="G130">
+        <v>1113</v>
+      </c>
+      <c r="H130">
+        <v>1110</v>
+      </c>
+      <c r="I130">
+        <v>690</v>
+      </c>
+      <c r="J130">
+        <v>602</v>
+      </c>
+      <c r="K130">
+        <v>1062</v>
+      </c>
+      <c r="L130">
+        <v>5068</v>
+      </c>
+      <c r="M130">
+        <v>728</v>
+      </c>
+      <c r="N130">
+        <v>1200</v>
+      </c>
+      <c r="O130">
+        <v>376</v>
+      </c>
+      <c r="P130">
+        <v>2887</v>
+      </c>
+      <c r="Q130">
+        <v>114</v>
+      </c>
+      <c r="R130">
+        <v>764</v>
+      </c>
+      <c r="S130">
+        <v>6373</v>
+      </c>
+      <c r="T130">
+        <v>387</v>
+      </c>
+      <c r="U130">
+        <v>5069</v>
+      </c>
+      <c r="V130">
+        <v>215</v>
+      </c>
+      <c r="W130">
+        <v>762</v>
+      </c>
+      <c r="X130">
+        <v>438</v>
+      </c>
+      <c r="Y130">
+        <v>2153</v>
+      </c>
+      <c r="Z130">
+        <v>741</v>
+      </c>
+      <c r="AA130">
+        <v>533</v>
+      </c>
+      <c r="AB130">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="131" spans="1:28">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>15996</v>
+      </c>
+      <c r="C131">
+        <v>1781</v>
+      </c>
+      <c r="D131">
+        <v>10624</v>
+      </c>
+      <c r="E131">
+        <v>2050</v>
+      </c>
+      <c r="F131">
+        <v>671</v>
+      </c>
+      <c r="G131">
+        <v>1134</v>
+      </c>
+      <c r="H131">
+        <v>1183</v>
+      </c>
+      <c r="I131">
+        <v>715</v>
+      </c>
+      <c r="J131">
+        <v>621</v>
+      </c>
+      <c r="K131">
+        <v>1082</v>
+      </c>
+      <c r="L131">
+        <v>5116</v>
+      </c>
+      <c r="M131">
+        <v>763</v>
+      </c>
+      <c r="N131">
+        <v>1213</v>
+      </c>
+      <c r="O131">
+        <v>383</v>
+      </c>
+      <c r="P131">
+        <v>2918</v>
+      </c>
+      <c r="Q131">
+        <v>117</v>
+      </c>
+      <c r="R131">
+        <v>783</v>
+      </c>
+      <c r="S131">
+        <v>6441</v>
+      </c>
+      <c r="T131">
+        <v>391</v>
+      </c>
+      <c r="U131">
+        <v>5096</v>
+      </c>
+      <c r="V131">
+        <v>220</v>
+      </c>
+      <c r="W131">
+        <v>784</v>
+      </c>
+      <c r="X131">
+        <v>441</v>
+      </c>
+      <c r="Y131">
+        <v>2185</v>
+      </c>
+      <c r="Z131">
+        <v>786</v>
+      </c>
+      <c r="AA131">
+        <v>548</v>
+      </c>
+      <c r="AB131">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="132" spans="1:28">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>16078</v>
+      </c>
+      <c r="C132">
+        <v>1803</v>
+      </c>
+      <c r="D132">
+        <v>10667</v>
+      </c>
+      <c r="E132">
+        <v>2107</v>
+      </c>
+      <c r="F132">
+        <v>699</v>
+      </c>
+      <c r="G132">
+        <v>1153</v>
+      </c>
+      <c r="H132">
+        <v>1201</v>
+      </c>
+      <c r="I132">
+        <v>727</v>
+      </c>
+      <c r="J132">
+        <v>621</v>
+      </c>
+      <c r="K132">
+        <v>1099</v>
+      </c>
+      <c r="L132">
+        <v>5143</v>
+      </c>
+      <c r="M132">
+        <v>795</v>
+      </c>
+      <c r="N132">
+        <v>1213</v>
+      </c>
+      <c r="O132">
+        <v>393</v>
+      </c>
+      <c r="P132">
+        <v>2929</v>
+      </c>
+      <c r="Q132">
+        <v>117</v>
+      </c>
+      <c r="R132">
+        <v>798</v>
+      </c>
+      <c r="S132">
+        <v>6441</v>
+      </c>
+      <c r="T132">
+        <v>391</v>
+      </c>
+      <c r="U132">
+        <v>5105</v>
+      </c>
+      <c r="V132">
+        <v>220</v>
+      </c>
+      <c r="W132">
+        <v>809</v>
+      </c>
+      <c r="X132">
+        <v>442</v>
+      </c>
+      <c r="Y132">
+        <v>2219</v>
+      </c>
+      <c r="Z132">
+        <v>821</v>
+      </c>
+      <c r="AA132">
+        <v>555</v>
+      </c>
+      <c r="AB132">
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -20138,15 +20838,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2">
         <v>1777225</v>
@@ -20154,7 +20854,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B3">
         <v>881935</v>
@@ -20162,7 +20862,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B4">
         <v>4144597</v>
@@ -20170,7 +20870,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B5">
         <v>605761</v>
@@ -20178,7 +20878,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B6">
         <v>8602865</v>
@@ -20186,7 +20886,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B7">
         <v>845731</v>
@@ -20194,7 +20894,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B8">
         <v>1572866</v>
@@ -20202,7 +20902,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B9">
         <v>7075181</v>
@@ -20210,7 +20910,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B10">
         <v>3273227</v>
@@ -20218,7 +20918,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B11">
         <v>9132078</v>
@@ -20226,7 +20926,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B12">
         <v>3506853</v>
@@ -20234,7 +20934,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B13">
         <v>4018127</v>
@@ -20242,7 +20942,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B14">
         <v>9557071</v>
@@ -20250,7 +20950,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B15">
         <v>3337357</v>
@@ -20258,7 +20958,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B16">
         <v>2298696</v>
@@ -20266,7 +20966,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B17">
         <v>14873064</v>
@@ -20274,7 +20974,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B18">
         <v>21168791</v>
@@ -20282,7 +20982,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B19">
         <v>4018650</v>
@@ -20290,7 +20990,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B20">
         <v>17264943</v>
@@ -20298,7 +20998,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B21">
         <v>45919049</v>
@@ -20306,7 +21006,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B22">
         <v>11433957</v>
@@ -20314,7 +21014,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B23">
         <v>7164788</v>
@@ -20322,7 +21022,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B24">
         <v>11377239</v>
@@ -20330,7 +21030,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B25">
         <v>2778986</v>
@@ -20338,7 +21038,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B26">
         <v>3484466</v>
@@ -20346,7 +21046,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B27">
         <v>7018354</v>
@@ -20354,7 +21054,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B28">
         <v>3015268</v>

</xml_diff>

<commit_message>
Updating plot ranges, breaks and labels
</commit_message>
<xml_diff>
--- a/data/Brasil.xlsx
+++ b/data/Brasil.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="163">
   <si>
     <t>2020-02-25</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t>2020-07-06</t>
+  </si>
+  <si>
+    <t>2020-07-07</t>
   </si>
   <si>
     <t>UF</t>
@@ -833,7 +836,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB133"/>
+  <dimension ref="A1:AB134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10867,7 +10870,7 @@
         <v>32769</v>
       </c>
       <c r="N133">
-        <v>35056</v>
+        <v>35809</v>
       </c>
       <c r="O133">
         <v>33822</v>
@@ -10876,7 +10879,7 @@
         <v>76427</v>
       </c>
       <c r="Q133">
-        <v>10253</v>
+        <v>10687</v>
       </c>
       <c r="R133">
         <v>30718</v>
@@ -10891,7 +10894,7 @@
         <v>116152</v>
       </c>
       <c r="V133">
-        <v>12640</v>
+        <v>13004</v>
       </c>
       <c r="W133">
         <v>27514</v>
@@ -10909,7 +10912,93 @@
         <v>23920</v>
       </c>
       <c r="AB133">
-        <v>18948</v>
+        <v>19088</v>
+      </c>
+    </row>
+    <row r="134" spans="1:28">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>332708</v>
+      </c>
+      <c r="C134">
+        <v>56703</v>
+      </c>
+      <c r="D134">
+        <v>124086</v>
+      </c>
+      <c r="E134">
+        <v>91954</v>
+      </c>
+      <c r="F134">
+        <v>62694</v>
+      </c>
+      <c r="G134">
+        <v>41524</v>
+      </c>
+      <c r="H134">
+        <v>60897</v>
+      </c>
+      <c r="I134">
+        <v>33800</v>
+      </c>
+      <c r="J134">
+        <v>32001</v>
+      </c>
+      <c r="K134">
+        <v>54802</v>
+      </c>
+      <c r="L134">
+        <v>66151</v>
+      </c>
+      <c r="M134">
+        <v>34308</v>
+      </c>
+      <c r="N134">
+        <v>35809</v>
+      </c>
+      <c r="O134">
+        <v>35343</v>
+      </c>
+      <c r="P134">
+        <v>79167</v>
+      </c>
+      <c r="Q134">
+        <v>10687</v>
+      </c>
+      <c r="R134">
+        <v>31640</v>
+      </c>
+      <c r="S134">
+        <v>126142</v>
+      </c>
+      <c r="T134">
+        <v>14941</v>
+      </c>
+      <c r="U134">
+        <v>118744</v>
+      </c>
+      <c r="V134">
+        <v>13004</v>
+      </c>
+      <c r="W134">
+        <v>28411</v>
+      </c>
+      <c r="X134">
+        <v>30294</v>
+      </c>
+      <c r="Y134">
+        <v>92088</v>
+      </c>
+      <c r="Z134">
+        <v>23506</v>
+      </c>
+      <c r="AA134">
+        <v>24563</v>
+      </c>
+      <c r="AB134">
+        <v>19088</v>
       </c>
     </row>
   </sheetData>
@@ -10919,7 +11008,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB133"/>
+  <dimension ref="A1:AB134"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -20953,7 +21042,7 @@
         <v>820</v>
       </c>
       <c r="N133">
-        <v>1254</v>
+        <v>1289</v>
       </c>
       <c r="O133">
         <v>406</v>
@@ -20962,7 +21051,7 @@
         <v>2938</v>
       </c>
       <c r="Q133">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="R133">
         <v>826</v>
@@ -20977,7 +21066,7 @@
         <v>5128</v>
       </c>
       <c r="V133">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="W133">
         <v>834</v>
@@ -20995,7 +21084,93 @@
         <v>558</v>
       </c>
       <c r="AB133">
-        <v>371</v>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="134" spans="1:28">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>16475</v>
+      </c>
+      <c r="C134">
+        <v>1879</v>
+      </c>
+      <c r="D134">
+        <v>10881</v>
+      </c>
+      <c r="E134">
+        <v>2216</v>
+      </c>
+      <c r="F134">
+        <v>767</v>
+      </c>
+      <c r="G134">
+        <v>1192</v>
+      </c>
+      <c r="H134">
+        <v>1282</v>
+      </c>
+      <c r="I134">
+        <v>793</v>
+      </c>
+      <c r="J134">
+        <v>726</v>
+      </c>
+      <c r="K134">
+        <v>1145</v>
+      </c>
+      <c r="L134">
+        <v>5234</v>
+      </c>
+      <c r="M134">
+        <v>851</v>
+      </c>
+      <c r="N134">
+        <v>1289</v>
+      </c>
+      <c r="O134">
+        <v>420</v>
+      </c>
+      <c r="P134">
+        <v>2952</v>
+      </c>
+      <c r="Q134">
+        <v>128</v>
+      </c>
+      <c r="R134">
+        <v>851</v>
+      </c>
+      <c r="S134">
+        <v>6563</v>
+      </c>
+      <c r="T134">
+        <v>399</v>
+      </c>
+      <c r="U134">
+        <v>5169</v>
+      </c>
+      <c r="V134">
+        <v>228</v>
+      </c>
+      <c r="W134">
+        <v>858</v>
+      </c>
+      <c r="X134">
+        <v>455</v>
+      </c>
+      <c r="Y134">
+        <v>2286</v>
+      </c>
+      <c r="Z134">
+        <v>896</v>
+      </c>
+      <c r="AA134">
+        <v>577</v>
+      </c>
+      <c r="AB134">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -21013,15 +21188,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B2">
         <v>1777225</v>
@@ -21029,7 +21204,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B3">
         <v>881935</v>
@@ -21037,7 +21212,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B4">
         <v>4144597</v>
@@ -21045,7 +21220,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B5">
         <v>605761</v>
@@ -21053,7 +21228,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B6">
         <v>8602865</v>
@@ -21061,7 +21236,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B7">
         <v>845731</v>
@@ -21069,7 +21244,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B8">
         <v>1572866</v>
@@ -21077,7 +21252,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B9">
         <v>7075181</v>
@@ -21085,7 +21260,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B10">
         <v>3273227</v>
@@ -21093,7 +21268,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B11">
         <v>9132078</v>
@@ -21101,7 +21276,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B12">
         <v>3506853</v>
@@ -21109,7 +21284,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B13">
         <v>4018127</v>
@@ -21117,7 +21292,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B14">
         <v>9557071</v>
@@ -21125,7 +21300,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B15">
         <v>3337357</v>
@@ -21133,7 +21308,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B16">
         <v>2298696</v>
@@ -21141,7 +21316,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B17">
         <v>14873064</v>
@@ -21149,7 +21324,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B18">
         <v>21168791</v>
@@ -21157,7 +21332,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B19">
         <v>4018650</v>
@@ -21165,7 +21340,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B20">
         <v>17264943</v>
@@ -21173,7 +21348,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B21">
         <v>45919049</v>
@@ -21181,7 +21356,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B22">
         <v>11433957</v>
@@ -21189,7 +21364,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B23">
         <v>7164788</v>
@@ -21197,7 +21372,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B24">
         <v>11377239</v>
@@ -21205,7 +21380,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B25">
         <v>2778986</v>
@@ -21213,7 +21388,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B26">
         <v>3484466</v>
@@ -21221,7 +21396,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B27">
         <v>7018354</v>
@@ -21229,7 +21404,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B28">
         <v>3015268</v>

</xml_diff>